<commit_message>
A few small adjustments to sim functions, trying to fix lack of novelrr mortality benefit but not sure i've fixed it. Also added ability to model RIF monoR outcomes.
</commit_message>
<xml_diff>
--- a/BPaMZ Xpert XDR cohort model parameters.xlsx
+++ b/BPaMZ Xpert XDR cohort model parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekendal2\OneDrive - Johns Hopkins University\Research\universal regimen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekendal2\Johns Hopkins University\OneDrive - Johns Hopkins University\Research\universal regimen\universal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="350">
   <si>
     <t>RIF-R</t>
   </si>
@@ -1187,6 +1187,9 @@
   </si>
   <si>
     <t>(data from ahuja as presented in who 2016 dr update)</t>
+  </si>
+  <si>
+    <t>Also assume that H(ZE) results in same outcomes as (ZE) or single novel drug since nothing to sterilize, with acquired INH-R</t>
   </si>
 </sst>
 </file>
@@ -1852,18 +1855,18 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="48" customWidth="1"/>
-    <col min="4" max="5" width="8.28515625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="48" customWidth="1"/>
+    <col min="4" max="5" width="8.33203125" style="48" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8 16384:16384" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8 16384:16384" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>91</v>
       </c>
@@ -2030,7 +2033,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>91</v>
       </c>
@@ -2051,7 +2054,7 @@
       </c>
       <c r="XFD8" s="6"/>
     </row>
-    <row r="9" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>90</v>
       </c>
@@ -2072,7 +2075,7 @@
       </c>
       <c r="XFD9" s="6"/>
     </row>
-    <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
@@ -2093,7 +2096,7 @@
       </c>
       <c r="XFD10" s="6"/>
     </row>
-    <row r="11" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2116,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -2171,7 +2174,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -2189,7 +2192,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>332</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>336</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>336</v>
       </c>
@@ -2251,21 +2254,21 @@
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="D20" s="52"/>
       <c r="E20" s="52"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>234</v>
       </c>
@@ -2274,7 +2277,7 @@
       <c r="E21" s="52"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2284,7 +2287,7 @@
       <c r="E22" s="52"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2294,7 +2297,7 @@
       <c r="E23" s="52"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2304,7 +2307,7 @@
       <c r="E24" s="52"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2323,15 +2326,15 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="63.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="63.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2371,7 +2374,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>218</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>209</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>214</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>303</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>304</v>
       </c>
@@ -2532,7 +2535,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>344</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>342</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>343</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2607,7 +2610,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>231</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>325</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>262</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>263</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>274</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>227</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0.88</v>
       </c>
@@ -2741,22 +2744,22 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="62" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="65" t="s">
         <v>279</v>
       </c>
@@ -2771,35 +2774,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="15" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" customWidth="1"/>
+    <col min="13" max="15" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>136</v>
       </c>
@@ -2808,27 +2811,27 @@
         <v>6.2780269058295965E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="66" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" s="7" t="s">
         <v>131</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>141</v>
       </c>
@@ -2884,12 +2887,12 @@
         <v>6.2789334729015683E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="55" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>131</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>142</v>
       </c>
@@ -2945,17 +2948,17 @@
         <v>2.3707165354241951E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>135</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>115</v>
       </c>
@@ -2994,7 +2997,7 @@
         <v>9.8039215686274508E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>117</v>
       </c>
@@ -3015,7 +3018,7 @@
         <v>1.4975041597337771E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>118</v>
       </c>
@@ -3036,7 +3039,7 @@
         <v>6.1349693251533744E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>119</v>
       </c>
@@ -3052,14 +3055,14 @@
       <c r="L24" s="54"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C26" s="59"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="59"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>154</v>
       </c>
@@ -3072,7 +3075,7 @@
         <v>0.18751497202801296</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>311</v>
       </c>
@@ -3085,7 +3088,7 @@
         <v>0.1853071819334916</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>312</v>
       </c>
@@ -3094,17 +3097,17 @@
         <v>0.24449366556290514</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>126</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>115</v>
       </c>
@@ -3138,7 +3141,7 @@
         <v>2.6876122082585283</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>117</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>2.563186813186813</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>118</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>306</v>
       </c>
@@ -3195,7 +3198,7 @@
         <v>2.6688834387261569</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>127</v>
       </c>
@@ -3207,7 +3210,7 @@
         <v>5.5859138528967699E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>129</v>
       </c>
@@ -3216,22 +3219,22 @@
         <v>0.16757741558690309</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>131</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>132</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>5.5845555508945446E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>133</v>
       </c>
@@ -3315,17 +3318,17 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="67" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="56" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>120</v>
       </c>
@@ -3333,7 +3336,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>100</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>101</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>103</v>
       </c>
@@ -3367,7 +3370,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>102</v>
       </c>
@@ -3379,7 +3382,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>282</v>
       </c>
@@ -3387,7 +3390,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>131</v>
       </c>
@@ -3410,7 +3413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>164</v>
       </c>
@@ -3442,7 +3445,7 @@
         <v>4.0538337629079137E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -3474,12 +3477,12 @@
         <v>5.3482202008838665E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
         <v>160</v>
       </c>
@@ -3487,7 +3490,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D69">
         <v>2</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>97</v>
       </c>
@@ -3554,7 +3557,7 @@
         <v>0.10870685213807318</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>98</v>
       </c>
@@ -3595,17 +3598,17 @@
         <v>0.26086956521739135</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>328</v>
       </c>
@@ -3613,7 +3616,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D76">
         <v>1</v>
       </c>
@@ -3633,7 +3636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>104</v>
       </c>
@@ -3656,7 +3659,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>105</v>
       </c>
@@ -3679,7 +3682,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>106</v>
       </c>
@@ -3702,7 +3705,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>108</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>109</v>
       </c>
@@ -3748,7 +3751,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>107</v>
       </c>
@@ -3771,17 +3774,17 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D86">
         <v>1</v>
       </c>
@@ -3801,7 +3804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>110</v>
       </c>
@@ -3824,7 +3827,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>111</v>
       </c>
@@ -3847,7 +3850,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>112</v>
       </c>
@@ -3870,7 +3873,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>113</v>
       </c>
@@ -3893,7 +3896,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>285</v>
       </c>
@@ -3916,208 +3919,213 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B92" s="67" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L104" s="7"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L105" s="62"/>
       <c r="M105" s="62"/>
       <c r="N105" s="62"/>
       <c r="O105" s="62"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L106" s="62"/>
       <c r="M106" s="62"/>
       <c r="N106" s="62"/>
       <c r="O106" s="62"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L107" s="62"/>
       <c r="M107" s="62"/>
       <c r="N107" s="62"/>
       <c r="O107" s="62"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L108" s="62"/>
       <c r="M108" s="62"/>
       <c r="N108" s="62"/>
       <c r="O108" s="62"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L109" s="62"/>
       <c r="M109" s="62"/>
       <c r="N109" s="62"/>
       <c r="O109" s="62"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L110" s="62"/>
       <c r="M110" s="62"/>
       <c r="N110" s="62"/>
       <c r="O110" s="62"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L111" s="62"/>
       <c r="M111" s="62"/>
       <c r="N111" s="62"/>
       <c r="O111" s="62"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L112" s="62"/>
       <c r="M112" s="62"/>
       <c r="N112" s="62"/>
       <c r="O112" s="62"/>
     </row>
-    <row r="113" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L113" s="62"/>
       <c r="M113" s="62"/>
       <c r="N113" s="62"/>
       <c r="O113" s="62"/>
     </row>
-    <row r="114" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L114" s="62"/>
       <c r="M114" s="62"/>
       <c r="N114" s="62"/>
       <c r="O114" s="62"/>
     </row>
-    <row r="115" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L115" s="62"/>
       <c r="M115" s="62"/>
       <c r="N115" s="62"/>
       <c r="O115" s="62"/>
     </row>
-    <row r="116" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L116" s="62"/>
       <c r="M116" s="62"/>
       <c r="N116" s="62"/>
       <c r="O116" s="62"/>
     </row>
-    <row r="117" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L117" s="62"/>
       <c r="M117" s="62"/>
       <c r="N117" s="62"/>
       <c r="O117" s="62"/>
     </row>
-    <row r="118" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L118" s="62"/>
       <c r="M118" s="62"/>
       <c r="N118" s="62"/>
       <c r="O118" s="62"/>
     </row>
-    <row r="119" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L119" s="62"/>
       <c r="M119" s="62"/>
       <c r="N119" s="62"/>
       <c r="O119" s="62"/>
     </row>
-    <row r="120" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L120" s="62"/>
       <c r="M120" s="62"/>
       <c r="N120" s="62"/>
       <c r="O120" s="62"/>
     </row>
-    <row r="121" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L121" s="62"/>
       <c r="M121" s="62"/>
       <c r="N121" s="62"/>
       <c r="O121" s="62"/>
     </row>
-    <row r="122" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L122" s="62"/>
       <c r="M122" s="62"/>
       <c r="N122" s="62"/>
       <c r="O122" s="62"/>
     </row>
-    <row r="123" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L123" s="62"/>
       <c r="M123" s="62"/>
       <c r="N123" s="62"/>
       <c r="O123" s="62"/>
     </row>
-    <row r="124" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L124" s="62"/>
       <c r="M124" s="62"/>
       <c r="N124" s="62"/>
       <c r="O124" s="62"/>
     </row>
-    <row r="125" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L125" s="62"/>
       <c r="M125" s="62"/>
       <c r="N125" s="62"/>
       <c r="O125" s="62"/>
     </row>
-    <row r="126" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L126" s="62"/>
       <c r="M126" s="62"/>
       <c r="N126" s="62"/>
       <c r="O126" s="62"/>
     </row>
-    <row r="127" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L127" s="62"/>
       <c r="M127" s="62"/>
       <c r="N127" s="62"/>
       <c r="O127" s="62"/>
     </row>
-    <row r="128" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L128" s="62"/>
       <c r="M128" s="62"/>
       <c r="N128" s="62"/>
       <c r="O128" s="62"/>
     </row>
-    <row r="129" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L129" s="62"/>
       <c r="M129" s="62"/>
       <c r="N129" s="62"/>
       <c r="O129" s="62"/>
     </row>
-    <row r="130" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L130" s="62"/>
       <c r="M130" s="62"/>
       <c r="N130" s="62"/>
       <c r="O130" s="62"/>
     </row>
-    <row r="131" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L131" s="62"/>
       <c r="M131" s="62"/>
       <c r="N131" s="62"/>
       <c r="O131" s="62"/>
     </row>
-    <row r="132" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L132" s="62"/>
       <c r="M132" s="62"/>
       <c r="N132" s="62"/>
       <c r="O132" s="62"/>
     </row>
-    <row r="133" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L133" s="62"/>
       <c r="M133" s="62"/>
       <c r="N133" s="62"/>
@@ -4137,14 +4145,14 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>207</v>
       </c>
@@ -4186,7 +4194,7 @@
       <c r="T2" s="62"/>
       <c r="U2" s="62"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -4209,7 +4217,7 @@
         <v>5.5845555508945446E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -4232,7 +4240,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -4255,7 +4263,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -4287,7 +4295,7 @@
         <v>0.10870685213807318</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>166</v>
       </c>
@@ -4319,7 +4327,7 @@
         <v>0.26086956521739135</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -4342,7 +4350,7 @@
         <v>2.9633956692802436E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -4365,7 +4373,7 @@
         <v>5.0672922036348919E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>101</v>
       </c>
@@ -4388,7 +4396,7 @@
         <v>6.685275251104833E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -4411,7 +4419,7 @@
         <v>6.685275251104833E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>103</v>
       </c>
@@ -4434,7 +4442,7 @@
         <v>6.685275251104833E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -4457,7 +4465,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -4480,7 +4488,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -4503,7 +4511,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -4526,7 +4534,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -4549,7 +4557,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -4572,7 +4580,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -4595,7 +4603,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -4618,7 +4626,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -4641,7 +4649,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>113</v>
       </c>
@@ -4664,7 +4672,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>167</v>
       </c>
@@ -4687,7 +4695,7 @@
         <v>5.5845555508945446E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>168</v>
       </c>
@@ -4710,7 +4718,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -4733,7 +4741,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4756,7 +4764,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>171</v>
       </c>
@@ -4779,7 +4787,7 @@
         <v>5.5845555508945446E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -4802,7 +4810,7 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>173</v>
       </c>
@@ -4834,7 +4842,7 @@
         <v>0.10870685213807318</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>174</v>
       </c>
@@ -4866,7 +4874,7 @@
         <v>0.26086956521739135</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>1</v>
       </c>
@@ -4899,63 +4907,63 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" customWidth="1"/>
-    <col min="2" max="5" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="65.6640625" customWidth="1"/>
+    <col min="2" max="5" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="62" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="62" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -4966,7 +4974,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>191</v>
       </c>
@@ -4977,7 +4985,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>192</v>
       </c>
@@ -4988,7 +4996,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>193</v>
       </c>
@@ -4999,7 +5007,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>194</v>
       </c>
@@ -5010,7 +5018,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>195</v>
       </c>
@@ -5021,17 +5029,17 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="62" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>181</v>
       </c>
@@ -5048,7 +5056,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -5059,7 +5067,7 @@
       <c r="D24" s="61"/>
       <c r="E24" s="61"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -5070,7 +5078,7 @@
       <c r="D25" s="61"/>
       <c r="E25" s="61"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>162</v>
       </c>
@@ -5079,7 +5087,7 @@
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>165</v>
       </c>
@@ -5090,7 +5098,7 @@
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -5099,7 +5107,7 @@
       <c r="D28" s="61"/>
       <c r="E28" s="61"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -5114,7 +5122,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -5129,7 +5137,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -5142,7 +5150,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -5155,7 +5163,7 @@
       </c>
       <c r="E32" s="61"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -5168,7 +5176,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -5181,7 +5189,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -5192,7 +5200,7 @@
       </c>
       <c r="E35" s="61"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -5205,7 +5213,7 @@
       </c>
       <c r="E36" s="61"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -5216,7 +5224,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -5229,7 +5237,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -5240,7 +5248,7 @@
       <c r="D39" s="61"/>
       <c r="E39" s="61"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -5251,7 +5259,7 @@
       </c>
       <c r="E40" s="61"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>111</v>
       </c>
@@ -5262,7 +5270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>112</v>
       </c>
@@ -5273,7 +5281,7 @@
       <c r="D42" s="61"/>
       <c r="E42" s="61"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>113</v>
       </c>
@@ -5282,7 +5290,7 @@
       <c r="D43" s="61"/>
       <c r="E43" s="61"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -5295,7 +5303,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>168</v>
       </c>
@@ -5306,7 +5314,7 @@
       </c>
       <c r="E45" s="61"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -5317,7 +5325,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -5326,7 +5334,7 @@
       <c r="D47" s="61"/>
       <c r="E47" s="61"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>171</v>
       </c>
@@ -5337,7 +5345,7 @@
       <c r="D48" s="61"/>
       <c r="E48" s="61"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>172</v>
       </c>
@@ -5348,7 +5356,7 @@
       <c r="D49" s="61"/>
       <c r="E49" s="61"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>173</v>
       </c>
@@ -5359,7 +5367,7 @@
       <c r="D50" s="61"/>
       <c r="E50" s="61"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>174</v>
       </c>
@@ -5368,17 +5376,17 @@
       <c r="D51" s="61"/>
       <c r="E51" s="61"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="67" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>330</v>
       </c>
@@ -5397,105 +5405,105 @@
       <selection activeCell="C31" sqref="B30:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
     <col min="4" max="5" width="28" customWidth="1"/>
-    <col min="6" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="6" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
       <c r="B4" s="63" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="63" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="63" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="63" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="63" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="63" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" s="63" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" s="63" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="63" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C17" s="63" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="64" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="63" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="63" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="63" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="62"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>253</v>
       </c>
@@ -5503,7 +5511,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>254</v>
       </c>
@@ -5511,7 +5519,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>294</v>
       </c>
@@ -5519,7 +5527,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>299</v>
       </c>
@@ -5527,7 +5535,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>289</v>
       </c>
@@ -5538,7 +5546,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>292</v>
       </c>
@@ -5546,12 +5554,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>253</v>
       </c>
@@ -5565,7 +5573,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="55">
         <v>0</v>
       </c>
@@ -5582,7 +5590,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="55" t="s">
         <v>267</v>
       </c>
@@ -5599,7 +5607,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="55" t="s">
         <v>269</v>
       </c>
@@ -5616,7 +5624,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="55" t="s">
         <v>270</v>
       </c>
@@ -5633,7 +5641,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="55" t="s">
         <v>272</v>
       </c>
@@ -5650,7 +5658,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="55">
         <v>3</v>
       </c>
@@ -5667,7 +5675,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="55">
         <v>4</v>
       </c>
@@ -5684,7 +5692,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="55">
         <v>5</v>
       </c>
@@ -5714,22 +5722,22 @@
       <selection activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="s">
         <v>35</v>
       </c>
@@ -5739,7 +5747,7 @@
       <c r="E1" s="75"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="76" t="s">
         <v>36</v>
       </c>
@@ -5749,7 +5757,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:13" s="12" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="12" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>37</v>
@@ -5765,7 +5773,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>41</v>
       </c>
@@ -5785,7 +5793,7 @@
       </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>42</v>
       </c>
@@ -5805,7 +5813,7 @@
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>43</v>
       </c>
@@ -5824,7 +5832,7 @@
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="78" t="s">
         <v>44</v>
       </c>
@@ -5841,7 +5849,7 @@
       <c r="J7" s="74"/>
       <c r="K7" s="74"/>
     </row>
-    <row r="8" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
       <c r="B8" s="10" t="s">
         <v>46</v>
@@ -5866,7 +5874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>41</v>
       </c>
@@ -5898,7 +5906,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>42</v>
       </c>
@@ -5930,7 +5938,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>43</v>
       </c>
@@ -5968,7 +5976,7 @@
         <v>1.2793796417649628E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -5976,7 +5984,7 @@
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="79" t="s">
         <v>50</v>
       </c>
@@ -5994,7 +6002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="76" t="s">
         <v>36</v>
       </c>
@@ -6009,7 +6017,7 @@
       <c r="J14" s="77"/>
       <c r="K14" s="77"/>
     </row>
-    <row r="15" spans="1:13" s="12" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="12" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>51</v>
@@ -6040,7 +6048,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>41</v>
       </c>
@@ -6069,7 +6077,7 @@
       <c r="J16" s="34"/>
       <c r="K16" s="36"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>42</v>
       </c>
@@ -6098,7 +6106,7 @@
       <c r="J17" s="34"/>
       <c r="K17" s="36"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>58</v>
       </c>
@@ -6138,7 +6146,7 @@
         <v>6.4866936546338641E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="74" t="s">
         <v>59</v>
       </c>
@@ -6154,7 +6162,7 @@
       <c r="K19" s="74"/>
       <c r="M19" s="50"/>
     </row>
-    <row r="20" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
       <c r="B20" s="32" t="s">
         <v>60</v>
@@ -6186,7 +6194,7 @@
       </c>
       <c r="M20" s="50"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
         <v>41</v>
       </c>
@@ -6216,7 +6224,7 @@
       <c r="K21" s="36"/>
       <c r="M21" s="50"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
         <v>42</v>
       </c>
@@ -6246,7 +6254,7 @@
       <c r="K22" s="36"/>
       <c r="M22" s="50"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>58</v>
       </c>
@@ -6286,7 +6294,7 @@
         <v>7.3979515250887529E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="74" t="s">
         <v>65</v>
       </c>
@@ -6302,7 +6310,7 @@
       <c r="K24" s="74"/>
       <c r="M24" s="50"/>
     </row>
-    <row r="25" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41"/>
       <c r="B25" s="32" t="s">
         <v>66</v>
@@ -6334,7 +6342,7 @@
       </c>
       <c r="M25" s="50"/>
     </row>
-    <row r="26" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
@@ -6364,7 +6372,7 @@
       <c r="K26" s="36"/>
       <c r="M26" s="50"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
@@ -6394,7 +6402,7 @@
       <c r="K27" s="36"/>
       <c r="M27" s="50"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>58</v>
       </c>
@@ -6434,7 +6442,7 @@
         <v>0.15492471633806465</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
         <v>67</v>
       </c>
@@ -6449,16 +6457,16 @@
       <c r="J29" s="46"/>
       <c r="K29" s="46"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G30" s="18"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G31" s="18"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G32" s="18"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -6467,17 +6475,17 @@
         <v>152.40499999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>71</v>
       </c>
@@ -6488,7 +6496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>73</v>
       </c>
@@ -6517,7 +6525,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -6554,7 +6562,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -6588,7 +6596,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -6627,7 +6635,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -6668,7 +6676,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -6709,7 +6717,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -6722,7 +6730,7 @@
         <v>7.7678491013431907</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -6735,7 +6743,7 @@
         <v>56.383924550671594</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>71</v>
       </c>
@@ -6746,7 +6754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -6778,7 +6786,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -6820,7 +6828,7 @@
         <v>0.1167459059693608</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -6862,7 +6870,7 @@
         <v>0.25092445853143158</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -6904,7 +6912,7 @@
         <v>8.7691494981510826E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -6946,7 +6954,7 @@
         <v>4.0147913365029056E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -6963,12 +6971,12 @@
       <c r="F52" s="49"/>
       <c r="G52" s="49"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>81</v>
       </c>
@@ -6979,7 +6987,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -6999,7 +7007,7 @@
         <v>5.1299507536188622E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>83</v>
       </c>
@@ -7016,7 +7024,7 @@
         <v>0.28752642706131076</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -7036,7 +7044,7 @@
         <v>3.5656895306859206E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>83</v>
       </c>
@@ -7053,7 +7061,7 @@
         <v>0.15223027718550106</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>147</v>
       </c>
@@ -7076,7 +7084,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>83</v>
       </c>
@@ -7096,7 +7104,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -7116,7 +7124,7 @@
         <v>8.4620550705171257E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Still optimizing for valid results, planning to make a few changes like HZE outcomes and M-Z res correlation, and south africa version of params, and sensitivity analysis code
</commit_message>
<xml_diff>
--- a/BPaMZ Xpert XDR cohort model parameters.xlsx
+++ b/BPaMZ Xpert XDR cohort model parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6480" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patient characteristics - SEA" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="353">
   <si>
     <t>RIF-R</t>
   </si>
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>Incidence:prevalence estimates, SEA (e.g. WHO 2016 Global TB report)</t>
-  </si>
-  <si>
-    <t>Tbdxtime_recurrence</t>
   </si>
   <si>
     <t>Source/assumptions</t>
@@ -1056,9 +1053,6 @@
     <t>Average in months, from start of active TB, for new TB patients who eventually present to care</t>
   </si>
   <si>
-    <t>Average in months, from start of TB recurrence (due to relapse or reinfection), for individuals with a history of TB who are eventually diagnosed again</t>
-  </si>
-  <si>
     <t>Unavoidableloss</t>
   </si>
   <si>
@@ -1190,6 +1184,21 @@
   </si>
   <si>
     <t>Also assume that H(ZE) results in same outcomes as (ZE) or single novel drug since nothing to sterilize, with acquired INH-R</t>
+  </si>
+  <si>
+    <t>Xpert_max</t>
+  </si>
+  <si>
+    <t>Maximum fraction of pulm TB that can access Xpert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa WHO global report 2018 ~68% of all prev treated tested for RR -&gt; .68/.89/.9 = __ of Xpert+ pulmonary cases. as an example of a country with moderate rosources that has tried to scale up nationally. India has goal of doing the same. </t>
+  </si>
+  <si>
+    <t>Relative time to re-diagnosis, from start of TB recurrence (due to relapse or reinfection), for individuals with a history of TB who are eventually diagnosed again</t>
+  </si>
+  <si>
+    <t>Tbdxtime_recurrenceratio</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +1994,7 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
@@ -2009,7 +2018,7 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
@@ -2029,7 +2038,7 @@
         <v>0.08</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -2050,7 +2059,7 @@
         <v>0.19</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="XFD8" s="6"/>
     </row>
@@ -2071,7 +2080,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="XFD9" s="6"/>
     </row>
@@ -2092,7 +2101,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="XFD10" s="6"/>
     </row>
@@ -2101,7 +2110,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C11" s="52">
         <v>8.5000000000000006E-2</v>
@@ -2121,7 +2130,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C12" s="52">
         <v>0.152</v>
@@ -2194,7 +2203,7 @@
     </row>
     <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>32</v>
@@ -2209,15 +2218,15 @@
         <v>0.04</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C17" s="48">
         <f>(4308+1272)/(13232+1272+3005)</f>
@@ -2230,15 +2239,15 @@
         <v>0.45</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C18" s="52">
         <f>(6540+1163)/(12508+1628+1163)</f>
@@ -2251,7 +2260,7 @@
         <v>0.64</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2270,7 +2279,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21" s="1"/>
       <c r="D21" s="52"/>
@@ -2320,10 +2329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,10 +2357,10 @@
         <v>20</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2368,7 +2377,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F3" t="s">
         <v>217</v>
@@ -2376,24 +2385,24 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>352</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B5">
         <v>0.1</v>
@@ -2405,10 +2414,10 @@
         <v>0.2</v>
       </c>
       <c r="E5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2428,7 +2437,7 @@
         <v>211</v>
       </c>
       <c r="F6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2448,7 +2457,7 @@
         <v>213</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2468,7 +2477,7 @@
         <v>215</v>
       </c>
       <c r="F8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2488,7 +2497,7 @@
         <v>216</v>
       </c>
       <c r="F9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2505,39 +2514,39 @@
         <v>0.02</v>
       </c>
       <c r="E10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11">
         <f>1/4/12</f>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12">
         <f>1/40/12</f>
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="E12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B13">
         <v>2E-3</v>
@@ -2549,12 +2558,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B14">
         <f>(408-86)/(462-137)</f>
@@ -2567,15 +2576,15 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B15">
         <v>0.63</v>
@@ -2587,7 +2596,7 @@
         <v>0.71</v>
       </c>
       <c r="E15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2604,15 +2613,15 @@
         <v>0.99</v>
       </c>
       <c r="E16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B17">
         <v>0.96</v>
@@ -2624,15 +2633,15 @@
         <v>0.995</v>
       </c>
       <c r="E17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F17" t="s">
         <v>232</v>
-      </c>
-      <c r="F17" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B18">
         <v>0.75</v>
@@ -2644,15 +2653,15 @@
         <v>0.86</v>
       </c>
       <c r="E18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F18" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19">
         <v>0.25</v>
@@ -2664,15 +2673,15 @@
         <v>0.4</v>
       </c>
       <c r="E19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B20">
         <v>0.7</v>
@@ -2684,15 +2693,15 @@
         <v>0.8</v>
       </c>
       <c r="E20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -2704,15 +2713,15 @@
         <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F21" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B22">
         <f>0.9/12</f>
@@ -2727,41 +2736,50 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>348</v>
+      </c>
       <c r="B23">
-        <v>0.88</v>
+        <v>0.85</v>
       </c>
       <c r="C23">
-        <v>0.79</v>
+        <v>0.7</v>
       </c>
       <c r="D23">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="62" t="s">
-        <v>275</v>
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>349</v>
+      </c>
+      <c r="F23" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>276</v>
+      <c r="A25" s="62" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="65" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="65" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2774,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
@@ -2789,7 +2807,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2955,7 +2973,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -3077,7 +3095,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C29">
         <f>C24/(E12/(1-C24))</f>
@@ -3090,7 +3108,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C30" s="67">
         <f>AVERAGE(C28:G28)</f>
@@ -3099,7 +3117,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -3182,7 +3200,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C38" s="67">
         <f>SUMPRODUCT(C35:C37,D35:D37)/SUM(D35:D37)</f>
@@ -3384,7 +3402,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D61" t="s">
         <v>134</v>
@@ -3479,7 +3497,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -3600,17 +3618,17 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D75" t="s">
         <v>161</v>
@@ -3776,7 +3794,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -3898,7 +3916,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D91" s="67">
         <v>0.8</v>
@@ -3921,37 +3939,37 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B92" s="67" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
@@ -4149,7 +4167,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -4935,7 +4953,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -5072,7 +5090,7 @@
         <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C25" s="61"/>
       <c r="D25" s="61"/>
@@ -5350,7 +5368,7 @@
         <v>172</v>
       </c>
       <c r="B49" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C49" s="61"/>
       <c r="D49" s="61"/>
@@ -5378,17 +5396,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="67" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -5416,83 +5434,83 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
       <c r="B4" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="63" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="63" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" s="63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" s="63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C17" s="63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -5500,77 +5518,77 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C27" t="s">
         <v>294</v>
-      </c>
-      <c r="C27" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>288</v>
+      </c>
+      <c r="B30" t="s">
         <v>289</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>290</v>
-      </c>
-      <c r="C30" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
+        <v>291</v>
+      </c>
+      <c r="C31" t="s">
         <v>292</v>
-      </c>
-      <c r="C31" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
+        <v>252</v>
+      </c>
+      <c r="C34" t="s">
         <v>253</v>
       </c>
-      <c r="C34" t="s">
-        <v>254</v>
-      </c>
       <c r="D34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -5578,84 +5596,84 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
+        <v>259</v>
+      </c>
+      <c r="C35" t="s">
         <v>260</v>
       </c>
-      <c r="C35" t="s">
-        <v>261</v>
-      </c>
       <c r="D35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="55" t="s">
+        <v>266</v>
+      </c>
+      <c r="B36" t="s">
+        <v>259</v>
+      </c>
+      <c r="C36" t="s">
         <v>267</v>
       </c>
-      <c r="B36" t="s">
-        <v>260</v>
-      </c>
-      <c r="C36" t="s">
-        <v>268</v>
-      </c>
       <c r="D36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="55" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B37" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C37" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" t="s">
         <v>270</v>
       </c>
-      <c r="B38" t="s">
-        <v>271</v>
-      </c>
       <c r="C38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="55" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E39" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -5663,16 +5681,16 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -5680,16 +5698,16 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E41" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -5697,16 +5715,16 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PZA moxi correlation, code for notifications calculations, maybe a few other small model modifications
</commit_message>
<xml_diff>
--- a/BPaMZ Xpert XDR cohort model parameters.xlsx
+++ b/BPaMZ Xpert XDR cohort model parameters.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekendal2\Johns Hopkins University\OneDrive - Johns Hopkins University\Research\universal regimen\universal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/ekendal2_jh_edu/Documents/Research/universal regimen/universal/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6480"/>
   </bookViews>
   <sheets>
-    <sheet name="Patient characteristics - SEA" sheetId="1" r:id="rId1"/>
+    <sheet name="Patient characteristics" sheetId="1" r:id="rId1"/>
     <sheet name="TB epi and clinical practice" sheetId="7" r:id="rId2"/>
     <sheet name="Treatment outcomes assumptions" sheetId="3" r:id="rId3"/>
     <sheet name="Relapseprobs" sheetId="10" r:id="rId4"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="370">
   <si>
     <t>RIF-R</t>
   </si>
@@ -53,30 +53,12 @@
     <t>Denominator</t>
   </si>
   <si>
-    <t>Setting and source</t>
-  </si>
-  <si>
     <t>Other regional data</t>
   </si>
   <si>
-    <t>Bangladesh 1.6% 2011, Pakistan 4.2% 2013, India 2.2 (1.9-2.6) based on subnationa surveys, ~2006</t>
-  </si>
-  <si>
-    <t>India DRS survey 2014-2016, and SEA global report 2016</t>
-  </si>
-  <si>
     <t>Additional notes</t>
   </si>
   <si>
-    <t>Will depend on recent extent of up-front DST, so wide tolerance on the low end</t>
-  </si>
-  <si>
-    <t>12% in India DRS survey, 13% estimate for SEA in WHO 2017</t>
-  </si>
-  <si>
-    <t>29 (22-36) bangladesh 2011 but presumably decreasing since as up-front detection improves; 16 pakistan (2015)</t>
-  </si>
-  <si>
     <t>Zignol, Pakistan 23 of 63; Bangladesh 41 of 103; India DRS, 72 of 307</t>
   </si>
   <si>
@@ -131,12 +113,6 @@
     <t>All</t>
   </si>
   <si>
-    <t>WHO SEA 2016 (see R code)</t>
-  </si>
-  <si>
-    <t>22% in India, &lt;10% in most SEA countries</t>
-  </si>
-  <si>
     <t>PZA resistance assumptions</t>
   </si>
   <si>
@@ -399,9 +375,6 @@
   </si>
   <si>
     <t xml:space="preserve">For BPaZ, results for labeled (with loading) and 200mg doses are averaged. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Averages of overnight and spot solid culture results. When no spot culture was performed (BPaM), extrapolates from the difference between overnight and spot sensitivity for other regimens, to a value (93%) similarly intermediate between BPaZ and BPaMZ (Z-s) outcomes. </t>
   </si>
   <si>
     <t>Assumed same as BPaZ, and this matches the 83-94% 2 mo culture conversion (low and high doses) from NC-002 pamz data</t>
@@ -820,9 +793,6 @@
   </si>
   <si>
     <t>Xpert_current_rerx</t>
-  </si>
-  <si>
-    <t>Global Report 2017, SEA, with increase since collection of those data</t>
   </si>
   <si>
     <t>Fraction of recurrent TB patients getting Xpert before retreatment at baseline</t>
@@ -1141,9 +1111,6 @@
     <t>HIV-</t>
   </si>
   <si>
-    <t>WHO global report, lower bound is if all 36% unknowns are HIV neg, upper is if their HIV prev is higher.</t>
-  </si>
-  <si>
     <t>Smearpos</t>
   </si>
   <si>
@@ -1192,13 +1159,97 @@
     <t>Maximum fraction of pulm TB that can access Xpert</t>
   </si>
   <si>
-    <t xml:space="preserve">South Africa WHO global report 2018 ~68% of all prev treated tested for RR -&gt; .68/.89/.9 = __ of Xpert+ pulmonary cases. as an example of a country with moderate rosources that has tried to scale up nationally. India has goal of doing the same. </t>
-  </si>
-  <si>
     <t>Relative time to re-diagnosis, from start of TB recurrence (due to relapse or reinfection), for individuals with a history of TB who are eventually diagnosed again</t>
   </si>
   <si>
     <t>Tbdxtime_recurrenceratio</t>
+  </si>
+  <si>
+    <t>12% in India, &lt;10% in most SEA countries</t>
+  </si>
+  <si>
+    <t>SEA in WHO global report 2018</t>
+  </si>
+  <si>
+    <t>Bangladesh 1.6% 2011, Pakistan 4.2% 2013, India 2.8% (2.3-3.5) in 2014-16 DRS, India 2.2 (1.9-2.6) based on subnationa surveys, ~2006</t>
+  </si>
+  <si>
+    <t>13% (4.3-25) estimate for SEA in WHO 2018</t>
+  </si>
+  <si>
+    <t>29 (22-36) bangladesh 2011 but presumably decreasing since as up-front detection improves; 16 pakistan (2015); 12 (10-13) for India DRS 2014-16</t>
+  </si>
+  <si>
+    <t>Will depend on recent extent of up-front DST, so wide tolerance on the low end but top end coming down with better detection relative to the 25% in 2018 global report</t>
+  </si>
+  <si>
+    <t>probably some correlation with pza-r but Alame IJTLD 2015 suggests it is weak, and small N, so assumed independence for now</t>
+  </si>
+  <si>
+    <t>WHO SEA 2017 notifcation data (see R code, bpamz_cohort_setup.R)</t>
+  </si>
+  <si>
+    <t>villellas…andries JAC 2017, 8/347 MDR (and 0.7% non-MDR) had Rv0678 variants with high MIC</t>
+  </si>
+  <si>
+    <t>WHO global report 2018 for SEA, lower bound is if all 45% unknowns are HIV neg, upper is if their HIV prev is higher.</t>
+  </si>
+  <si>
+    <t>S Af</t>
+  </si>
+  <si>
+    <t>Setting and source, SEA</t>
+  </si>
+  <si>
+    <t>Source, Saf</t>
+  </si>
+  <si>
+    <t>see same R code</t>
+  </si>
+  <si>
+    <t>Zignol, both SA sites</t>
+  </si>
+  <si>
+    <t>Zignol, weighted average of 2 SA sites</t>
+  </si>
+  <si>
+    <t>Zignol, weighted average of 2 SA sites, 0.5ug/ml</t>
+  </si>
+  <si>
+    <t>http://www.nicd.ac.za/assets/files/K-12750%20NICD%20National%20Survey%20Report_Dev_V11-LR.pdf</t>
+  </si>
+  <si>
+    <t>Glboal report 2018</t>
+  </si>
+  <si>
+    <t>as for SEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Averages of overnight and spot solid culture results. When no spot culture was performed (BPaM), extrapolates from the difference between overnight and spot sensitivity for other regimens, to a value similarly intermediate between BPaZ and BPaMZ (Z-s) outcomes. </t>
+  </si>
+  <si>
+    <t>Global Report 2018, SEA, with increase since collection of those data</t>
+  </si>
+  <si>
+    <t>Global Report 2018, SEA, with projected increase to 2019 assume 2017-18 trend continues</t>
+  </si>
+  <si>
+    <t>South Africa WHO global report 2018 ~68% of all prev treated tested for RR -&gt; .68/.89/.9 = __ of Xpert+ pulmonary cases. as an example of a country with moderate rosources that has tried to scale up nationally. India has goal of doing the same. Assume can push slightly higher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similarly for rifampin monoresistance H(ZE), no sterilizing drug so don't follow same time scales. </t>
+  </si>
+  <si>
+    <t>In Fox W IJTLD 1999 at https://www.ingentaconnect.com/contentone/iuatld/ijtld/1999/00000003/A00210s2/art00001#, 77% 2 mo culture conversion, and 18% relapse after 6 mo rx. i.e. wallis model doesn't apply (no sterilizing drug), so take same approach as for MDR, using relapse rate at 9 months (5%) and scaling duration in log term by 1.5</t>
+  </si>
+  <si>
+    <t>H(ZE)</t>
+  </si>
+  <si>
+    <t>OR-PZA-if-MOXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IJTLD 2015 Alame-Emane , among RR 10 PZA only, 12 PZA and FQ, 24 neither, 10 FQ only. </t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1261,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1322,6 +1373,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF3C4043"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1409,7 +1466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1566,6 +1623,7 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1577,6 +1635,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1858,10 +1918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,13 +1929,13 @@
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="48" customWidth="1"/>
-    <col min="4" max="5" width="8.33203125" style="48" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="4" max="7" width="8.33203125" style="48" customWidth="1"/>
+    <col min="8" max="8" width="42.109375" customWidth="1"/>
+    <col min="9" max="9" width="34.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8 16384:16384" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -1883,76 +1943,92 @@
         <v>6</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>351</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C2" s="48">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="48">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E2" s="48">
-        <v>0.22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+        <v>0.13</v>
+      </c>
+      <c r="F2" s="48">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="H2" t="s">
+        <v>348</v>
+      </c>
+      <c r="I2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3" s="52">
-        <v>2.8000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D3" s="52">
-        <v>0.02</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E3" s="52">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F3" s="52">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G3" s="52"/>
+      <c r="H3" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="52">
         <v>0.13</v>
@@ -1963,17 +2039,21 @@
       <c r="E4" s="52">
         <v>0.2</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F4" s="52">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G4" s="52"/>
+      <c r="H4" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1989,15 +2069,21 @@
       <c r="E5" s="52">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F5" s="52">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>355</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2013,17 +2099,24 @@
       <c r="E6" s="53">
         <v>0.4</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F6" s="53">
+        <f>(0.391*39+0.491*34)/(39+34)</f>
+        <v>0.43757534246575341</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -2037,14 +2130,22 @@
       <c r="E7" s="52">
         <v>0.08</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F7" s="52">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="J7" s="65" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -2058,14 +2159,20 @@
       <c r="E8" s="52">
         <v>0.19</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="XFD8" s="6"/>
-    </row>
-    <row r="9" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F8" s="52">
+        <f>(0.084*41+0.122*33)/(41+33)</f>
+        <v>0.10094594594594596</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -2079,14 +2186,19 @@
       <c r="E9" s="52">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="XFD9" s="6"/>
-    </row>
-    <row r="10" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F9" s="52">
+        <v>2E-3</v>
+      </c>
+      <c r="G9" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -2100,17 +2212,23 @@
       <c r="E10" s="52">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="XFD10" s="6"/>
-    </row>
-    <row r="11" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F10" s="52">
+        <f>0.038*40/(40+31)</f>
+        <v>2.1408450704225351E-2</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>356</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C11" s="52">
         <v>8.5000000000000006E-2</v>
@@ -2121,16 +2239,23 @@
       <c r="E11" s="52">
         <v>0.1</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F11" s="48">
+        <f>(7.6-2.1)/(100-2.1)</f>
+        <v>5.6179775280898875E-2</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C12" s="52">
         <v>0.152</v>
@@ -2141,11 +2266,18 @@
       <c r="E12" s="52">
         <v>0.18</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F12" s="52">
+        <f>(11.1-4.6)/(100-4.6)</f>
+        <v>6.8134171907756808E-2</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2161,16 +2293,23 @@
       <c r="E13" s="52">
         <v>1</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="F13" s="52">
+        <f>((2.1)/3.4 +4.6/7.1)/2</f>
+        <v>0.63276719138359572</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>358</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C14" s="52">
         <v>0</v>
@@ -2179,54 +2318,66 @@
         <v>0</v>
       </c>
       <c r="E14" s="52">
-        <v>0.01</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="F14" s="52">
+        <v>0</v>
+      </c>
+      <c r="G14" s="52"/>
+      <c r="H14" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C15" s="52">
         <v>0</v>
       </c>
-      <c r="D15" s="52">
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52">
         <v>0</v>
       </c>
-      <c r="E15" s="52">
-        <v>0.01</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:8 16384:16384" x14ac:dyDescent="0.3">
+      <c r="G15" s="52"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C16" s="48">
-        <v>0.03</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D16" s="52">
-        <v>0.02</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E16" s="52">
-        <v>0.04</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="52">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C17" s="48">
         <f>(4308+1272)/(13232+1272+3005)</f>
@@ -2238,16 +2389,22 @@
       <c r="E17" s="52">
         <v>0.45</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="52">
+        <v>0.45</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>360</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C18" s="52">
         <f>(6540+1163)/(12508+1628+1163)</f>
@@ -2259,66 +2416,106 @@
       <c r="E18" s="52">
         <v>0.64</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="52">
+        <v>0.64</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>360</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="B20" s="1"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="C20" s="82">
+        <f>(12*24)/(10*10)</f>
+        <v>2.88</v>
+      </c>
+      <c r="D20" s="83">
+        <v>0.01</v>
+      </c>
+      <c r="E20" s="83">
+        <v>0.08</v>
+      </c>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52" t="s">
+        <v>369</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="D21" s="52"/>
       <c r="E21" s="52"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>23</v>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="52"/>
       <c r="D22" s="52"/>
       <c r="E22" s="52"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="52"/>
       <c r="D23" s="52"/>
       <c r="E23" s="52"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="52"/>
       <c r="D24" s="52"/>
       <c r="E24" s="52"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2331,8 +2528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,24 +2545,24 @@
         <v>5</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -2377,15 +2574,15 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -2397,12 +2594,12 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B5">
         <v>0.1</v>
@@ -2414,15 +2611,15 @@
         <v>0.2</v>
       </c>
       <c r="E5" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="F5" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2434,15 +2631,15 @@
         <v>0.5</v>
       </c>
       <c r="E6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F6" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2454,15 +2651,15 @@
         <v>0.1</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>0.25</v>
@@ -2474,15 +2671,15 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F8" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B9">
         <v>0.05</v>
@@ -2494,15 +2691,15 @@
         <v>0.2</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F9" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>0.01</v>
@@ -2514,39 +2711,55 @@
         <v>0.02</v>
       </c>
       <c r="E10" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B11">
         <f>1/4/12</f>
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="C11">
+        <f>1/7/12</f>
+        <v>1.1904761904761904E-2</v>
+      </c>
+      <c r="D11">
+        <f>1/3/12</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="E11" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B12">
         <f>1/40/12</f>
         <v>2.0833333333333333E-3</v>
       </c>
+      <c r="C12">
+        <f>1/50/12</f>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="D12">
+        <f>1/30/12</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
       <c r="E12" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B13">
         <v>2E-3</v>
@@ -2558,12 +2771,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E13" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B14">
         <f>(408-86)/(462-137)</f>
@@ -2576,15 +2789,15 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="F14" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B15">
         <v>0.63</v>
@@ -2596,12 +2809,12 @@
         <v>0.71</v>
       </c>
       <c r="E15" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>0.95</v>
@@ -2613,15 +2826,15 @@
         <v>0.99</v>
       </c>
       <c r="E16" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F16" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B17">
         <v>0.96</v>
@@ -2633,15 +2846,15 @@
         <v>0.995</v>
       </c>
       <c r="E17" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F17" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B18">
         <v>0.75</v>
@@ -2653,55 +2866,55 @@
         <v>0.86</v>
       </c>
       <c r="E18" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="F18" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B19">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="C19">
-        <v>0.15</v>
+        <v>0.27</v>
       </c>
       <c r="D19">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E19" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="F19" t="s">
-        <v>263</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B20">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C20">
-        <v>0.66</v>
+        <v>0.85</v>
       </c>
       <c r="D20">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="E20" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F20" t="s">
-        <v>263</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -2713,15 +2926,15 @@
         <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F21" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B22">
         <f>0.9/12</f>
@@ -2736,50 +2949,50 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E22" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F22" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="B23">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="C23">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="F23" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="62" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="65" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2790,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O133"/>
+  <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2807,22 +3020,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C4" s="67">
         <f>(26+53+5)/(502+676+160)</f>
@@ -2831,27 +3044,27 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="66" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2874,7 +3087,7 @@
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C12" s="70">
         <f>0.846</f>
@@ -2907,12 +3120,12 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="55" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2935,7 +3148,7 @@
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C16">
         <f>1-0.0178</f>
@@ -2968,34 +3181,34 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C21">
         <v>0.16400000000000001</v>
@@ -3017,7 +3230,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C22">
         <v>0.16700000000000001</v>
@@ -3038,7 +3251,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C23">
         <v>7.5999999999999998E-2</v>
@@ -3059,7 +3272,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C24" s="59">
         <f>SUMPRODUCT(C21:C23,$D21:$D23)/SUM($D21:$D23)</f>
@@ -3082,7 +3295,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C28">
         <f>C24/E12</f>
@@ -3095,7 +3308,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C29">
         <f>C24/(E12/(1-C24))</f>
@@ -3108,7 +3321,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C30" s="67">
         <f>AVERAGE(C28:G28)</f>
@@ -3117,23 +3330,23 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F34" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="G34" t="s">
         <v>4</v>
@@ -3141,7 +3354,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C35">
         <f>29/(470+29)</f>
@@ -3161,7 +3374,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <f>53/622</f>
@@ -3181,7 +3394,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -3200,7 +3413,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="C38" s="67">
         <f>SUMPRODUCT(C35:C37,D35:D37)/SUM(D35:D37)</f>
@@ -3218,10 +3431,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C40" s="72">
         <f>F38*I12</f>
@@ -3230,7 +3443,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C41" s="72">
         <f>G38*I12</f>
@@ -3239,22 +3452,22 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -3277,7 +3490,7 @@
     </row>
     <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C49">
         <v>0.87939999999999996</v>
@@ -3309,7 +3522,7 @@
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D50" s="57">
         <f>MIN(1,3*D49)</f>
@@ -3338,79 +3551,79 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="67" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="56" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C56" s="68">
         <v>0.94</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C57" s="68">
         <v>0.88500000000000001</v>
       </c>
       <c r="D57" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C58" s="68">
         <f>C57</f>
         <v>0.88500000000000001</v>
       </c>
       <c r="D58" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C59" s="68">
         <f>C57</f>
         <v>0.88500000000000001</v>
       </c>
       <c r="D59" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D61" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3433,7 +3646,7 @@
     </row>
     <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C63">
         <v>0.94</v>
@@ -3465,7 +3678,7 @@
     </row>
     <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C64">
         <v>0.89</v>
@@ -3497,15 +3710,15 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D68" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
@@ -3536,7 +3749,7 @@
     </row>
     <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C70" s="69">
         <f>(1-(890+840)/(979+962))</f>
@@ -3577,7 +3790,7 @@
     </row>
     <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C71" s="69">
         <f>(1-(72+81)/(95+112))</f>
@@ -3618,160 +3831,87 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>346</v>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>283</v>
+      <c r="B74" s="74" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>326</v>
-      </c>
-      <c r="D75" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76">
+      <c r="B75" t="s">
+        <v>367</v>
+      </c>
+      <c r="C75" s="67">
+        <v>0.05</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:I75" si="7">MIN(1,$C75/$I$49*(EXP(2.5289-2.5018*LN(D$69/1.5)+0.4399*LN((1-$C49)/($C49)))/(1+EXP(2.5289-2.5018*LN(D$69/1.5)+0.4399*LN((1-$C49)/($C49))))))</f>
+        <v>0.64296008864774701</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="7"/>
+        <v>0.42994687550549765</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="7"/>
+        <v>0.27778194815653057</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="7"/>
+        <v>0.18327313441093826</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="7"/>
+        <v>0.12555958414963159</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="7"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>316</v>
+      </c>
+      <c r="D80" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
         <v>2</v>
       </c>
-      <c r="F76">
+      <c r="F81">
         <v>3</v>
       </c>
-      <c r="G76">
+      <c r="G81">
         <v>4</v>
       </c>
-      <c r="H76">
+      <c r="H81">
         <v>5</v>
       </c>
-      <c r="I76">
+      <c r="I81">
         <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77">
-        <v>1</v>
-      </c>
-      <c r="F77">
-        <v>0.75283185383108231</v>
-      </c>
-      <c r="G77">
-        <v>0.42071668357850145</v>
-      </c>
-      <c r="H77">
-        <v>0.25609995471661978</v>
-      </c>
-      <c r="I77">
-        <v>0.16753666652683635</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
-        <v>105</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78">
-        <v>0.75283185383108231</v>
-      </c>
-      <c r="G78">
-        <v>0.42071668357850145</v>
-      </c>
-      <c r="H78">
-        <v>0.25609995471661978</v>
-      </c>
-      <c r="I78">
-        <v>0.16753666652683635</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>106</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79">
-        <v>0.75283185383108231</v>
-      </c>
-      <c r="G79">
-        <v>0.42071668357850145</v>
-      </c>
-      <c r="H79">
-        <v>0.25609995471661978</v>
-      </c>
-      <c r="I79">
-        <v>0.16753666652683635</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>108</v>
-      </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>1</v>
-      </c>
-      <c r="F80">
-        <v>0.75283185383108231</v>
-      </c>
-      <c r="G80">
-        <v>0.42071668357850145</v>
-      </c>
-      <c r="H80">
-        <v>0.25609995471661978</v>
-      </c>
-      <c r="I80">
-        <v>0.16753666652683635</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
-        <v>109</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-      <c r="E81">
-        <v>1</v>
-      </c>
-      <c r="F81">
-        <v>0.75283185383108231</v>
-      </c>
-      <c r="G81">
-        <v>0.42071668357850145</v>
-      </c>
-      <c r="H81">
-        <v>0.25609995471661978</v>
-      </c>
-      <c r="I81">
-        <v>0.16753666652683635</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -3792,218 +3932,303 @@
         <v>0.16753666652683635</v>
       </c>
     </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>0.75283185383108231</v>
+      </c>
+      <c r="G83">
+        <v>0.42071668357850145</v>
+      </c>
+      <c r="H83">
+        <v>0.25609995471661978</v>
+      </c>
+      <c r="I83">
+        <v>0.16753666652683635</v>
+      </c>
+    </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>327</v>
+      <c r="B84" t="s">
+        <v>98</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>0.75283185383108231</v>
+      </c>
+      <c r="G84">
+        <v>0.42071668357850145</v>
+      </c>
+      <c r="H84">
+        <v>0.25609995471661978</v>
+      </c>
+      <c r="I84">
+        <v>0.16753666652683635</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D85" t="s">
-        <v>161</v>
+      <c r="B85" t="s">
+        <v>100</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>0.75283185383108231</v>
+      </c>
+      <c r="G85">
+        <v>0.42071668357850145</v>
+      </c>
+      <c r="H85">
+        <v>0.25609995471661978</v>
+      </c>
+      <c r="I85">
+        <v>0.16753666652683635</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>101</v>
+      </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86">
-        <v>3</v>
+        <v>0.75283185383108231</v>
       </c>
       <c r="G86">
-        <v>4</v>
+        <v>0.42071668357850145</v>
       </c>
       <c r="H86">
-        <v>5</v>
+        <v>0.25609995471661978</v>
       </c>
       <c r="I86">
-        <v>6</v>
+        <v>0.16753666652683635</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>110</v>
-      </c>
-      <c r="D87" s="67">
+        <v>99</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>0.75283185383108231</v>
+      </c>
+      <c r="G87">
+        <v>0.42071668357850145</v>
+      </c>
+      <c r="H87">
+        <v>0.25609995471661978</v>
+      </c>
+      <c r="I87">
+        <v>0.16753666652683635</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>5</v>
+      </c>
+      <c r="I91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92" s="67">
         <v>0.8</v>
       </c>
-      <c r="E87" s="67">
+      <c r="E92" s="67">
         <v>0.8</v>
       </c>
-      <c r="F87" s="67">
+      <c r="F92" s="67">
         <v>0.8</v>
       </c>
-      <c r="G87" s="67">
+      <c r="G92" s="67">
         <v>0.8</v>
       </c>
-      <c r="H87" s="67">
+      <c r="H92" s="67">
         <v>0.8</v>
       </c>
-      <c r="I87" s="67">
+      <c r="I92" s="67">
         <v>0.8</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
-        <v>111</v>
-      </c>
-      <c r="D88" s="67">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+      <c r="D93" s="67">
         <v>0.8</v>
       </c>
-      <c r="E88" s="67">
+      <c r="E93" s="67">
         <v>0.8</v>
       </c>
-      <c r="F88" s="67">
+      <c r="F93" s="67">
         <v>0.8</v>
       </c>
-      <c r="G88" s="67">
+      <c r="G93" s="67">
         <v>0.8</v>
       </c>
-      <c r="H88" s="67">
+      <c r="H93" s="67">
         <v>0.8</v>
       </c>
-      <c r="I88" s="67">
+      <c r="I93" s="67">
         <v>0.8</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
-        <v>112</v>
-      </c>
-      <c r="D89" s="67">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>104</v>
+      </c>
+      <c r="D94" s="67">
         <v>0.8</v>
       </c>
-      <c r="E89" s="67">
+      <c r="E94" s="67">
         <v>0.8</v>
       </c>
-      <c r="F89" s="67">
+      <c r="F94" s="67">
         <v>0.8</v>
       </c>
-      <c r="G89" s="67">
+      <c r="G94" s="67">
         <v>0.8</v>
       </c>
-      <c r="H89" s="67">
+      <c r="H94" s="67">
         <v>0.8</v>
       </c>
-      <c r="I89" s="67">
+      <c r="I94" s="67">
         <v>0.8</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
-        <v>113</v>
-      </c>
-      <c r="D90" s="67">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>105</v>
+      </c>
+      <c r="D95" s="67">
         <v>0.8</v>
       </c>
-      <c r="E90" s="67">
+      <c r="E95" s="67">
         <v>0.8</v>
       </c>
-      <c r="F90" s="67">
+      <c r="F95" s="67">
         <v>0.8</v>
       </c>
-      <c r="G90" s="67">
+      <c r="G95" s="67">
         <v>0.8</v>
       </c>
-      <c r="H90" s="67">
+      <c r="H95" s="67">
         <v>0.8</v>
       </c>
-      <c r="I90" s="67">
+      <c r="I95" s="67">
         <v>0.8</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
-        <v>284</v>
-      </c>
-      <c r="D91" s="67">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>274</v>
+      </c>
+      <c r="D96" s="67">
         <v>0.8</v>
       </c>
-      <c r="E91" s="67">
+      <c r="E96" s="67">
         <v>0.8</v>
       </c>
-      <c r="F91" s="67">
+      <c r="F96" s="67">
         <v>0.8</v>
       </c>
-      <c r="G91" s="67">
+      <c r="G96" s="67">
         <v>0.8</v>
       </c>
-      <c r="H91" s="67">
+      <c r="H96" s="67">
         <v>0.8</v>
       </c>
-      <c r="I91" s="67">
+      <c r="I96" s="67">
         <v>0.8</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B92" s="67" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>316</v>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B97" s="67" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L104" s="7"/>
+      <c r="A104" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L105" s="62"/>
-      <c r="M105" s="62"/>
-      <c r="N105" s="62"/>
-      <c r="O105" s="62"/>
+      <c r="A105" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L106" s="62"/>
-      <c r="M106" s="62"/>
-      <c r="N106" s="62"/>
-      <c r="O106" s="62"/>
+      <c r="A106" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L107" s="62"/>
-      <c r="M107" s="62"/>
-      <c r="N107" s="62"/>
-      <c r="O107" s="62"/>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L108" s="62"/>
-      <c r="M108" s="62"/>
-      <c r="N108" s="62"/>
-      <c r="O108" s="62"/>
+      <c r="A107" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L109" s="62"/>
-      <c r="M109" s="62"/>
-      <c r="N109" s="62"/>
-      <c r="O109" s="62"/>
+      <c r="L109" s="7"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L110" s="62"/>
@@ -4148,6 +4373,36 @@
       <c r="M133" s="62"/>
       <c r="N133" s="62"/>
       <c r="O133" s="62"/>
+    </row>
+    <row r="134" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L134" s="62"/>
+      <c r="M134" s="62"/>
+      <c r="N134" s="62"/>
+      <c r="O134" s="62"/>
+    </row>
+    <row r="135" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L135" s="62"/>
+      <c r="M135" s="62"/>
+      <c r="N135" s="62"/>
+      <c r="O135" s="62"/>
+    </row>
+    <row r="136" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L136" s="62"/>
+      <c r="M136" s="62"/>
+      <c r="N136" s="62"/>
+      <c r="O136" s="62"/>
+    </row>
+    <row r="137" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L137" s="62"/>
+      <c r="M137" s="62"/>
+      <c r="N137" s="62"/>
+      <c r="O137" s="62"/>
+    </row>
+    <row r="138" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L138" s="62"/>
+      <c r="M138" s="62"/>
+      <c r="N138" s="62"/>
+      <c r="O138" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4167,12 +4422,12 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B2" s="62">
         <v>1</v>
@@ -4214,7 +4469,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B3">
         <v>0.83955543634544316</v>
@@ -4237,7 +4492,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4260,7 +4515,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4283,7 +4538,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4315,7 +4570,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4347,7 +4602,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>0.85294997005919293</v>
@@ -4370,7 +4625,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B9">
         <v>0.98616496672624221</v>
@@ -4393,7 +4648,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4416,7 +4671,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4439,7 +4694,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4462,7 +4717,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -4485,7 +4740,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4508,7 +4763,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4531,7 +4786,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4554,7 +4809,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4577,7 +4832,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4600,7 +4855,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4623,7 +4878,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4646,7 +4901,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -4669,7 +4924,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4692,7 +4947,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B23">
         <v>0.83955543634544316</v>
@@ -4715,7 +4970,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4738,7 +4993,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4761,7 +5016,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4784,7 +5039,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B27">
         <v>0.83955543634544316</v>
@@ -4807,7 +5062,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4830,7 +5085,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4862,7 +5117,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4921,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4933,153 +5188,153 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="62" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="62" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B14">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B15" s="1">
         <v>2E-3</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B16" s="1">
         <v>0.04</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B19" s="1">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="62" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C24" s="61"/>
       <c r="D24" s="61"/>
@@ -5087,10 +5342,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C25" s="61"/>
       <c r="D25" s="61"/>
@@ -5098,7 +5353,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B26" s="61"/>
       <c r="C26" s="61"/>
@@ -5107,18 +5362,18 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B27" s="61"/>
       <c r="C27" s="60" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B28" s="61"/>
       <c r="C28" s="61"/>
@@ -5127,148 +5382,148 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B29" s="61"/>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D29" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E29" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B30" s="61"/>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B31" s="61"/>
       <c r="C31" s="61"/>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E31" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B32" s="61"/>
       <c r="C32" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D32" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E32" s="61"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B33" s="61"/>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D33" s="61"/>
       <c r="E33" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B34" s="61"/>
       <c r="C34" s="61"/>
       <c r="D34" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E34" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B35" s="61"/>
       <c r="C35" s="61"/>
       <c r="D35" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E35" s="61"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B36" s="61"/>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E36" s="61"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B37" s="61"/>
       <c r="C37" s="61"/>
       <c r="D37" s="61"/>
       <c r="E37" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B38" s="61"/>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D38" s="61"/>
       <c r="E38" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B39" s="61"/>
       <c r="C39" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D39" s="61"/>
       <c r="E39" s="61"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B40" s="61"/>
       <c r="C40" s="61"/>
@@ -5279,7 +5534,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -5290,7 +5545,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="60">
@@ -5301,7 +5556,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
@@ -5310,42 +5565,42 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B44" s="61"/>
       <c r="C44" s="61"/>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E45" s="61"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B46" s="61"/>
       <c r="C46" s="61"/>
       <c r="D46" s="61"/>
       <c r="E46" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B47" s="61"/>
       <c r="C47" s="61"/>
@@ -5354,10 +5609,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C48" s="61"/>
       <c r="D48" s="61"/>
@@ -5365,10 +5620,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C49" s="61"/>
       <c r="D49" s="61"/>
@@ -5376,18 +5631,18 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B50" s="61"/>
       <c r="C50" s="60" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D50" s="61"/>
       <c r="E50" s="61"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B51" s="61"/>
       <c r="C51" s="61"/>
@@ -5396,17 +5651,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="67" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -5434,83 +5689,83 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
       <c r="B4" s="63" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="63" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="63" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="63" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="63" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" s="63" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" s="63" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" s="63" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="63" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C17" s="63" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="64" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="63" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="63" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="63" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -5518,77 +5773,77 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C27" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C28" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B30" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="C30" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C31" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C34" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D34" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -5596,84 +5851,84 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C35" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="D35" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E35" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="55" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B36" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C36" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D36" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E36" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="55" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B37" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C37" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D37" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E37" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="55" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B38" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D38" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="E38" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="55" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B39" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C39" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D39" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="E39" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -5681,16 +5936,16 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C40" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D40" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E40" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -5698,16 +5953,16 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C41" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D41" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E41" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -5715,16 +5970,16 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C42" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D42" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E42" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -5737,7 +5992,7 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5756,44 +6011,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="A1" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
+      <c r="A2" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="12" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B4" s="14">
         <v>751</v>
@@ -5813,7 +6068,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B5" s="14">
         <v>1299</v>
@@ -5833,7 +6088,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B6" s="19">
         <f>SUM(B4:B5)</f>
@@ -5851,50 +6106,50 @@
       <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
+      <c r="A7" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
+      <c r="G7" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
     </row>
     <row r="8" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
       <c r="B8" s="10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="24"/>
       <c r="H8" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I8" s="25"/>
       <c r="J8" s="10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B9" s="26">
         <v>63</v>
@@ -5909,7 +6164,7 @@
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H9" s="26">
         <v>892</v>
@@ -5926,7 +6181,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B10" s="26">
         <v>103</v>
@@ -5941,7 +6196,7 @@
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H10" s="26">
         <v>1397</v>
@@ -5958,7 +6213,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B11" s="20">
         <f t="shared" ref="B11:C11" si="0">SUM(B9:B10)</f>
@@ -5978,7 +6233,7 @@
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H11" s="20">
         <f t="shared" ref="H11" si="1">SUM(H9:H10)</f>
@@ -6003,72 +6258,72 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
+      <c r="A13" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
       <c r="M13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
+      <c r="A14" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
     </row>
     <row r="15" spans="1:13" s="12" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="32" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K15" s="32" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B16" s="14">
         <v>732</v>
@@ -6097,7 +6352,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B17" s="14">
         <v>1299</v>
@@ -6126,7 +6381,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B18" s="19">
         <f>SUM(B16:B17)</f>
@@ -6165,56 +6420,56 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
+      <c r="A19" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
       <c r="M19" s="50"/>
     </row>
     <row r="20" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
       <c r="B20" s="32" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="32" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H20" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="32" t="s">
-        <v>62</v>
-      </c>
       <c r="J20" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="32" t="s">
         <v>56</v>
-      </c>
-      <c r="K20" s="32" t="s">
-        <v>64</v>
       </c>
       <c r="M20" s="50"/>
     </row>
     <row r="21" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B21" s="34">
         <v>869</v>
@@ -6244,7 +6499,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B22" s="34">
         <v>1401</v>
@@ -6274,7 +6529,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B23" s="42">
         <f>SUM(B21:B22)</f>
@@ -6313,56 +6568,56 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
+      <c r="A24" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
       <c r="M24" s="50"/>
     </row>
     <row r="25" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41"/>
       <c r="B25" s="32" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="I25" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="32" t="s">
-        <v>62</v>
-      </c>
       <c r="J25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="32" t="s">
         <v>56</v>
-      </c>
-      <c r="K25" s="32" t="s">
-        <v>64</v>
       </c>
       <c r="M25" s="50"/>
     </row>
     <row r="26" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B26" s="34">
         <v>56</v>
@@ -6392,7 +6647,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B27" s="34">
         <v>100</v>
@@ -6422,7 +6677,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B28" s="42">
         <f>SUM(B26:B27)</f>
@@ -6462,7 +6717,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B29" s="46"/>
       <c r="C29" s="46"/>
@@ -6486,7 +6741,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="K33" s="47">
         <f>I23+D23</f>
@@ -6495,57 +6750,57 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I37" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="J38" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="K38" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B39">
         <f>C39+D39</f>
@@ -6582,7 +6837,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B40">
         <f>C40+D40</f>
@@ -6616,7 +6871,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B41">
         <f>C41+D41</f>
@@ -6655,7 +6910,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B42">
         <f>C42+D42</f>
@@ -6696,7 +6951,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B43">
         <f>C43+D43</f>
@@ -6737,7 +6992,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B44">
         <f>M28*B43</f>
@@ -6750,7 +7005,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B45">
         <f>(B44+B43)/2</f>
@@ -6763,50 +7018,50 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E46" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I46" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F47" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G47" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I47" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="J47" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="K47" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B48" s="48">
         <f t="shared" ref="B48:G52" si="3">B40/B$39</f>
@@ -6848,7 +7103,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B49" s="48">
         <f t="shared" si="3"/>
@@ -6890,7 +7145,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B50" s="48">
         <f t="shared" si="3"/>
@@ -6932,7 +7187,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B51" s="48">
         <f t="shared" si="3"/>
@@ -6974,7 +7229,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B52" s="48">
         <f t="shared" si="3"/>
@@ -6991,26 +7246,26 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" t="s">
         <v>81</v>
-      </c>
-      <c r="C56" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C57" s="47">
         <f>(D4+D5+E42)</f>
@@ -7027,7 +7282,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C58" s="47">
         <f>(D9+D10+B42)</f>
@@ -7044,10 +7299,10 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C59" s="47">
         <f>(I23+E43)</f>
@@ -7064,7 +7319,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C60" s="47">
         <f>(I28+B43)</f>
@@ -7081,10 +7336,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C61">
         <f>(D23+M23*E43)</f>
@@ -7099,12 +7354,12 @@
         <v>2.6367358909613046E-3</v>
       </c>
       <c r="F61" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C62">
         <f>(D28+M28*B43)</f>
@@ -7119,15 +7374,15 @@
         <v>2.3624699388559899E-2</v>
       </c>
       <c r="F62" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C63" s="47">
         <f>F41</f>
@@ -7144,7 +7399,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C64">
         <f>G41</f>

</xml_diff>

<commit_message>
Deep into analysis Jan 2019, finishing BPaMZ impact and starting DST impact
</commit_message>
<xml_diff>
--- a/BPaMZ Xpert XDR cohort model parameters.xlsx
+++ b/BPaMZ Xpert XDR cohort model parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/ekendal2_jh_edu/Documents/Research/universal regimen/universal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekendal2\Johns Hopkins University\OneDrive - Johns Hopkins University\Research\universal regimen\universal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1624,6 +1624,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1635,8 +1637,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1921,7 +1921,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1984,7 +1984,7 @@
         <v>0.13</v>
       </c>
       <c r="F2" s="48">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="G2" s="48" t="s">
         <v>354</v>
@@ -2441,14 +2441,14 @@
         <v>368</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="82">
+      <c r="C20" s="75">
         <f>(12*24)/(10*10)</f>
         <v>2.88</v>
       </c>
-      <c r="D20" s="83">
+      <c r="D20" s="76">
         <v>0.01</v>
       </c>
-      <c r="E20" s="83">
+      <c r="E20" s="76">
         <v>0.08</v>
       </c>
       <c r="F20" s="52"/>
@@ -3005,8 +3005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5176,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6011,23 +6011,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
       <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:13" s="12" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -6106,21 +6106,21 @@
       <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="23"/>
-      <c r="G7" s="79" t="s">
+      <c r="G7" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
     </row>
     <row r="8" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
@@ -6258,37 +6258,37 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
       <c r="M13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
     </row>
     <row r="15" spans="1:13" s="12" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
@@ -6420,19 +6420,19 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
       <c r="M19" s="50"/>
     </row>
     <row r="20" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6568,19 +6568,19 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
       <c r="M24" s="50"/>
     </row>
     <row r="25" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>